<commit_message>
tìm hiểu về bug
</commit_message>
<xml_diff>
--- a/Testcase_mvcprj.xlsx
+++ b/Testcase_mvcprj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -80,8 +80,34 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="MS PGothic"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="161">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -597,6 +623,12 @@
   </si>
   <si>
     <t>3. Không có tên đăng nhập này trong cơ sở dữ liệu.</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Register</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1521,6 +1553,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,23 +1604,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1602,96 +1718,38 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2057,13 +2115,13 @@
     </row>
     <row r="2" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -2077,11 +2135,11 @@
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
@@ -2093,36 +2151,36 @@
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="78" t="str">
+      <c r="C6" s="83" t="str">
         <f>C5&amp;"_"&amp;"XXX"&amp;"_"&amp;"vx.x"</f>
         <v>prj2_XXX_vx.x</v>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="85"/>
       <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="77"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
       <c r="F7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2303,11 +2361,11 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27"/>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="28"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -2318,39 +2376,39 @@
       <c r="F3" s="28"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="86" t="str">
+      <c r="C4" s="78"/>
+      <c r="D4" s="94" t="str">
         <f>Cover!C4</f>
         <v>MVC project (website tin tức)</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="88"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
     </row>
     <row r="5" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="86" t="str">
+      <c r="C5" s="78"/>
+      <c r="D5" s="94" t="str">
         <f>Cover!C5</f>
         <v>prj2</v>
       </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="88"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="92"/>
     </row>
     <row r="6" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="89" t="s">
+      <c r="C6" s="79"/>
+      <c r="D6" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="88"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="44"/>
@@ -2520,7 +2578,7 @@
     <mergeCell ref="D5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D10">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(D10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2541,9 +2599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,10 +2619,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="106"/>
+      <c r="B1" s="101"/>
       <c r="C1" s="60" t="s">
         <v>43</v>
       </c>
@@ -2580,16 +2638,16 @@
       <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="116" t="s">
+      <c r="B2" s="103"/>
+      <c r="C2" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="117"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="47"/>
       <c r="H2" s="48"/>
       <c r="I2" s="48"/>
@@ -2599,10 +2657,10 @@
       <c r="M2" s="42"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="103"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="50"/>
@@ -2616,10 +2674,10 @@
       <c r="M3" s="42"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="110"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="59" t="s">
         <v>48</v>
       </c>
@@ -2643,11 +2701,11 @@
       <c r="M4" s="56"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="111">
+      <c r="A5" s="106">
         <f>COUNTIF(J7:J24,"pass")</f>
         <v>15</v>
       </c>
-      <c r="B5" s="112"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="65">
         <f>COUNTIF(J10:J24,"fail")</f>
         <v>2</v>
@@ -2714,7 +2772,7 @@
       <c r="A7" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="118" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="70" t="s">
@@ -2734,7 +2792,7 @@
         <v>68</v>
       </c>
       <c r="I7" s="70"/>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K7" s="70"/>
@@ -2744,8 +2802,8 @@
       <c r="A8" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="93" t="s">
+      <c r="B8" s="119"/>
+      <c r="C8" s="121" t="s">
         <v>96</v>
       </c>
       <c r="D8" s="70" t="s">
@@ -2762,7 +2820,7 @@
         <v>73</v>
       </c>
       <c r="I8" s="70"/>
-      <c r="J8" s="113" t="s">
+      <c r="J8" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K8" s="70"/>
@@ -2772,8 +2830,8 @@
       <c r="A9" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="91"/>
-      <c r="C9" s="94"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="122"/>
       <c r="D9" s="70" t="s">
         <v>74</v>
       </c>
@@ -2788,7 +2846,7 @@
         <v>68</v>
       </c>
       <c r="I9" s="70"/>
-      <c r="J9" s="126"/>
+      <c r="J9" s="76"/>
       <c r="K9" s="70"/>
       <c r="L9" s="70"/>
     </row>
@@ -2796,8 +2854,8 @@
       <c r="A10" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="95"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="123"/>
       <c r="D10" s="70" t="s">
         <v>76</v>
       </c>
@@ -2810,7 +2868,7 @@
         <v>68</v>
       </c>
       <c r="I10" s="70"/>
-      <c r="J10" s="113" t="s">
+      <c r="J10" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K10" s="70"/>
@@ -2820,14 +2878,14 @@
       <c r="A11" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="99"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="102" t="s">
+      <c r="E11" s="108" t="s">
         <v>100</v>
       </c>
       <c r="F11" s="70" t="s">
@@ -2838,7 +2896,7 @@
         <v>102</v>
       </c>
       <c r="I11" s="70"/>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K11" s="70"/>
@@ -2848,12 +2906,12 @@
       <c r="A12" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="100"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="103"/>
+      <c r="E12" s="109"/>
       <c r="F12" s="70" t="s">
         <v>103</v>
       </c>
@@ -2862,7 +2920,7 @@
         <v>104</v>
       </c>
       <c r="I12" s="70"/>
-      <c r="J12" s="113" t="s">
+      <c r="J12" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K12" s="70"/>
@@ -2872,12 +2930,12 @@
       <c r="A13" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="98"/>
-      <c r="C13" s="101"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="104"/>
+      <c r="E13" s="110"/>
       <c r="F13" s="70" t="s">
         <v>105</v>
       </c>
@@ -2886,7 +2944,7 @@
         <v>133</v>
       </c>
       <c r="I13" s="70"/>
-      <c r="J13" s="113" t="s">
+      <c r="J13" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K13" s="70"/>
@@ -2896,16 +2954,16 @@
       <c r="A14" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="115" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="95" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="102" t="s">
+      <c r="E14" s="108" t="s">
         <v>135</v>
       </c>
       <c r="F14" s="70" t="s">
@@ -2918,7 +2976,7 @@
         <v>112</v>
       </c>
       <c r="I14" s="70"/>
-      <c r="J14" s="113" t="s">
+      <c r="J14" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K14" s="70"/>
@@ -2928,12 +2986,12 @@
       <c r="A15" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="100"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="103"/>
+      <c r="E15" s="109"/>
       <c r="F15" s="70" t="s">
         <v>124</v>
       </c>
@@ -2944,7 +3002,7 @@
         <v>130</v>
       </c>
       <c r="I15" s="70"/>
-      <c r="J15" s="113" t="s">
+      <c r="J15" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K15" s="70"/>
@@ -2954,12 +3012,12 @@
       <c r="A16" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="100"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="103"/>
+      <c r="E16" s="109"/>
       <c r="F16" s="70" t="s">
         <v>125</v>
       </c>
@@ -2970,7 +3028,7 @@
         <v>117</v>
       </c>
       <c r="I16" s="70"/>
-      <c r="J16" s="113" t="s">
+      <c r="J16" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K16" s="70"/>
@@ -2980,12 +3038,12 @@
       <c r="A17" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="100"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="111"/>
       <c r="D17" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="103"/>
+      <c r="E17" s="109"/>
       <c r="F17" s="70" t="s">
         <v>126</v>
       </c>
@@ -2996,7 +3054,7 @@
         <v>129</v>
       </c>
       <c r="I17" s="70"/>
-      <c r="J17" s="113" t="s">
+      <c r="J17" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K17" s="70"/>
@@ -3006,12 +3064,12 @@
       <c r="A18" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="100"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="111"/>
       <c r="D18" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="103"/>
+      <c r="E18" s="109"/>
       <c r="F18" s="70" t="s">
         <v>127</v>
       </c>
@@ -3022,7 +3080,7 @@
         <v>129</v>
       </c>
       <c r="I18" s="70"/>
-      <c r="J18" s="113" t="s">
+      <c r="J18" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K18" s="70"/>
@@ -3032,12 +3090,12 @@
       <c r="A19" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="120"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="96"/>
       <c r="D19" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="E19" s="104"/>
+      <c r="E19" s="110"/>
       <c r="F19" s="70" t="s">
         <v>128</v>
       </c>
@@ -3050,7 +3108,7 @@
       <c r="I19" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="J19" s="114" t="s">
+      <c r="J19" s="73" t="s">
         <v>132</v>
       </c>
       <c r="K19" s="70"/>
@@ -3060,14 +3118,14 @@
       <c r="A20" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="120"/>
+      <c r="B20" s="116"/>
       <c r="C20" s="70" t="s">
         <v>134</v>
       </c>
       <c r="D20" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="118" t="s">
+      <c r="E20" s="74" t="s">
         <v>135</v>
       </c>
       <c r="F20" s="70" t="s">
@@ -3080,7 +3138,7 @@
         <v>138</v>
       </c>
       <c r="I20" s="70"/>
-      <c r="J20" s="113" t="s">
+      <c r="J20" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K20" s="70"/>
@@ -3090,12 +3148,12 @@
       <c r="A21" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="121"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="70"/>
       <c r="D21" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="74" t="s">
         <v>135</v>
       </c>
       <c r="F21" s="70" t="s">
@@ -3106,7 +3164,7 @@
         <v>141</v>
       </c>
       <c r="I21" s="70"/>
-      <c r="J21" s="113" t="s">
+      <c r="J21" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K21" s="70"/>
@@ -3116,7 +3174,7 @@
       <c r="A22" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="123" t="s">
+      <c r="B22" s="97" t="s">
         <v>142</v>
       </c>
       <c r="C22" s="70" t="s">
@@ -3125,7 +3183,7 @@
       <c r="D22" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="122" t="s">
+      <c r="E22" s="75" t="s">
         <v>151</v>
       </c>
       <c r="F22" s="70" t="s">
@@ -3140,7 +3198,7 @@
       <c r="I22" s="70" t="s">
         <v>148</v>
       </c>
-      <c r="J22" s="114" t="s">
+      <c r="J22" s="73" t="s">
         <v>132</v>
       </c>
       <c r="K22" s="70"/>
@@ -3150,14 +3208,14 @@
       <c r="A23" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="99" t="s">
+      <c r="B23" s="98"/>
+      <c r="C23" s="95" t="s">
         <v>149</v>
       </c>
       <c r="D23" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="122" t="s">
+      <c r="E23" s="75" t="s">
         <v>150</v>
       </c>
       <c r="F23" s="70" t="s">
@@ -3170,7 +3228,7 @@
         <v>153</v>
       </c>
       <c r="I23" s="70"/>
-      <c r="J23" s="113" t="s">
+      <c r="J23" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K23" s="70"/>
@@ -3180,12 +3238,12 @@
       <c r="A24" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="101"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="70" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="122" t="s">
+      <c r="E24" s="75" t="s">
         <v>155</v>
       </c>
       <c r="F24" s="70" t="s">
@@ -3198,7 +3256,7 @@
         <v>158</v>
       </c>
       <c r="I24" s="70"/>
-      <c r="J24" s="113" t="s">
+      <c r="J24" s="72" t="s">
         <v>69</v>
       </c>
       <c r="K24" s="70"/>
@@ -4760,13 +4818,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="C14:C19"/>
     <mergeCell ref="C2:F2"/>
@@ -4776,12 +4827,19 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="E11:E13"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="K1:K5 J6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4796,14 +4854,692 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="127" customWidth="1"/>
+    <col min="2" max="16384" width="25.7109375" style="127"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="100" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="103"/>
+      <c r="C2" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="42"/>
+    </row>
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="103"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="42"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="104" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="105"/>
+      <c r="C4" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="56"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="106">
+        <f>COUNTIF(K7:K24,"pass")</f>
+        <v>0</v>
+      </c>
+      <c r="B5" s="107"/>
+      <c r="C5" s="65">
+        <f>COUNTIF(K10:K24,"fail")</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="66">
+        <f>COUNTBLANK(K7:K24)</f>
+        <v>18</v>
+      </c>
+      <c r="E5" s="67">
+        <f>COUNTIF(K10:K24,"N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="68">
+        <f>COUNTA(A7:A24)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="56"/>
+    </row>
+    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="128"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="128"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="128"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="128"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="128"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="128"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="128"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="128"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="128"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="128"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
+      <c r="M12" s="128"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="128"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="128"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="128"/>
+      <c r="M14" s="128"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="128"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="128"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="128"/>
+      <c r="L16" s="128"/>
+      <c r="M16" s="128"/>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="128"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="128"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="128"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="128"/>
+      <c r="L17" s="128"/>
+      <c r="M17" s="128"/>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="128"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="128"/>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="128"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="128"/>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="128"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="128"/>
+      <c r="L20" s="128"/>
+      <c r="M20" s="128"/>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="128"/>
+      <c r="B21" s="128"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
+      <c r="I21" s="128"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="128"/>
+      <c r="L21" s="128"/>
+      <c r="M21" s="128"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="128"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="128"/>
+      <c r="K22" s="128"/>
+      <c r="L22" s="128"/>
+      <c r="M22" s="128"/>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="128"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="128"/>
+      <c r="L23" s="128"/>
+      <c r="M23" s="128"/>
+    </row>
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="128"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="128"/>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="128"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="128"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="128"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="128"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="128"/>
+      <c r="M28" s="128"/>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="128"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
+      <c r="H29" s="128"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="128"/>
+      <c r="L29" s="128"/>
+      <c r="M29" s="128"/>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="128"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="128"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
+      <c r="L30" s="128"/>
+      <c r="M30" s="128"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="128"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="128"/>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
+      <c r="H31" s="128"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="128"/>
+      <c r="L31" s="128"/>
+      <c r="M31" s="128"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="128"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="128"/>
+      <c r="I32" s="128"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="128"/>
+      <c r="L32" s="128"/>
+      <c r="M32" s="128"/>
+    </row>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="128"/>
+      <c r="B33" s="128"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="128"/>
+      <c r="L33" s="128"/>
+      <c r="M33" s="128"/>
+    </row>
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="128"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="128"/>
+      <c r="L34" s="128"/>
+      <c r="M34" s="128"/>
+    </row>
+    <row r="35" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="128"/>
+      <c r="B35" s="128"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="128"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="128"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="128"/>
+    </row>
+    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="128"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="128"/>
+      <c r="J36" s="128"/>
+      <c r="K36" s="128"/>
+      <c r="L36" s="128"/>
+      <c r="M36" s="128"/>
+    </row>
+    <row r="37" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="128"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
+      <c r="E37" s="128"/>
+      <c r="F37" s="128"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="128"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="128"/>
+      <c r="L37" s="128"/>
+      <c r="M37" s="128"/>
+    </row>
+    <row r="38" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="128"/>
+      <c r="B38" s="128"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="128"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="128"/>
+      <c r="H38" s="128"/>
+      <c r="I38" s="128"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="128"/>
+      <c r="L38" s="128"/>
+      <c r="M38" s="128"/>
+    </row>
+    <row r="39" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="128"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
+      <c r="H39" s="128"/>
+      <c r="I39" s="128"/>
+      <c r="J39" s="128"/>
+      <c r="K39" s="128"/>
+      <c r="L39" s="128"/>
+      <c r="M39" s="128"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L1:L5 K6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="K6 L1:L2">
+      <formula1>$P$2:$P$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>